<commit_message>
fix all the things! Hopefully it works now.
</commit_message>
<xml_diff>
--- a/inst/loadExample.xlsx
+++ b/inst/loadExample.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Rprojects\openxlsx\inst\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="630" yWindow="555" windowWidth="17895" windowHeight="7365"/>
+    <workbookView xWindow="630" yWindow="555" windowWidth="17895" windowHeight="7365" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Heights and Widths" sheetId="5" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <sheet name="Chart" sheetId="6" r:id="rId4"/>
     <sheet name="Sales" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -840,6 +845,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -864,17 +880,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -885,6 +890,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -905,7 +913,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1026,94 +1033,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>9.6431458692483915E-2</c:v>
+                  <c:v>-1.6286369514996046</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.84422440654607145</c:v>
+                  <c:v>-0.80259671105381813</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.18511820778663166</c:v>
+                  <c:v>2.3434032378212764</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2.3402558711290427</c:v>
+                  <c:v>-0.76008968312749581</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.57025793151964643</c:v>
+                  <c:v>0.95598261500164772</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.95337537833018382</c:v>
+                  <c:v>0.45853959488243146</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6761834119742376</c:v>
+                  <c:v>-0.65981418430203442</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.41962809033921822</c:v>
+                  <c:v>1.0056392600088764</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.1555461732531676</c:v>
+                  <c:v>1.4267779198476243</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0324502986536035</c:v>
+                  <c:v>0.88625156403185001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-2.8545901234486373E-2</c:v>
+                  <c:v>0.47626721173020048</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.48755124380840653</c:v>
+                  <c:v>0.62298367675079713</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.18241007590871416</c:v>
+                  <c:v>-0.57811926669034175</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.40645151130854779</c:v>
+                  <c:v>-0.35823610365033776</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-1.8311490842109572</c:v>
+                  <c:v>-0.61238002422732263</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.96215492498844646</c:v>
+                  <c:v>-0.18649925450699487</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.3995494340984942</c:v>
+                  <c:v>0.81974219397416348</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.429627205651838</c:v>
+                  <c:v>0.27356123235836988</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.46732579014128267</c:v>
+                  <c:v>-0.64030197339033079</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.53704066915857618</c:v>
+                  <c:v>-0.59971385965600577</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-2.1793919844635887</c:v>
+                  <c:v>6.6845541758186314E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.1105943031094816</c:v>
+                  <c:v>0.45603723181899752</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.0122479941224252</c:v>
+                  <c:v>1.0509898886439115</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-1.2253461744283378</c:v>
+                  <c:v>-1.4983382337419218</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.95486093194605204</c:v>
+                  <c:v>1.7146782835268835</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.25488180096545371</c:v>
+                  <c:v>2.1833898119136865</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.87952993905620658</c:v>
+                  <c:v>0.31201518133058126</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.0472122627582323</c:v>
+                  <c:v>-1.3109688270183557</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.14803438285067375</c:v>
+                  <c:v>-1.9294154638738026</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.1002787723627714E-2</c:v>
+                  <c:v>-0.97504759908101213</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1128,11 +1135,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="82859136"/>
-        <c:axId val="82860672"/>
+        <c:axId val="177559520"/>
+        <c:axId val="177560080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82859136"/>
+        <c:axId val="177559520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1142,12 +1149,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82860672"/>
+        <c:crossAx val="177560080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82860672"/>
+        <c:axId val="177560080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1158,14 +1165,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82859136"/>
+        <c:crossAx val="177559520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1257,8 +1263,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="82949248"/>
-        <c:axId val="82950784"/>
+        <c:axId val="177562880"/>
+        <c:axId val="177563440"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1320,11 +1326,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="82954112"/>
-        <c:axId val="82952576"/>
+        <c:axId val="177564560"/>
+        <c:axId val="177564000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82949248"/>
+        <c:axId val="177562880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,7 +1339,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82950784"/>
+        <c:crossAx val="177563440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1341,7 +1347,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82950784"/>
+        <c:axId val="177563440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1352,12 +1358,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82949248"/>
+        <c:crossAx val="177562880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82952576"/>
+        <c:axId val="177564000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1367,12 +1373,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82954112"/>
+        <c:crossAx val="177564560"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="82954112"/>
+        <c:axId val="177564560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1381,7 +1387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82952576"/>
+        <c:crossAx val="177564000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1391,7 +1397,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1473,8 +1478,17 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
+            <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+              <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a14:imgLayer r:embed="rId3">
+                  <a14:imgEffect>
+                    <a14:colorTemperature colorTemp="6874"/>
+                  </a14:imgEffect>
+                </a14:imgLayer>
+              </a14:imgProps>
+            </a:ext>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
@@ -1492,6 +1506,15 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:glow rad="12700">
+            <a:schemeClr val="accent1">
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+          <a:reflection blurRad="825500" stA="47000" endPos="65000" dist="76200" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
+        </a:effectLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1795,7 +1818,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1830,7 +1853,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2041,7 +2064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2067,55 +2090,55 @@
       <c r="B15" t="s">
         <v>104</v>
       </c>
-      <c r="D15" s="82"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="82"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D16" s="83"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="85"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="90"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="83"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="85"/>
+      <c r="D17" s="88"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="90"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="83"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="85"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="91"/>
+      <c r="F18" s="90"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="83"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="85"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="90"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="83"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="85"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="90"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="83"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="85"/>
+      <c r="D21" s="88"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="90"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D22" s="83"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="85"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="90"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="94" t="s">
+      <c r="D26" s="86" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2138,11 +2161,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2153,19 +2176,19 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
     </row>
@@ -8583,7 +8606,7 @@
       </c>
       <c r="B1">
         <f ca="1">_xlfn.NORM.INV(RAND(), 0, 1)</f>
-        <v>9.6431458692483915E-2</v>
+        <v>-1.6286369514996046</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -8592,7 +8615,7 @@
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B30" ca="1" si="0">_xlfn.NORM.INV(RAND(), 0, 1)</f>
-        <v>0.84422440654607145</v>
+        <v>-0.80259671105381813</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -8601,7 +8624,7 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.18511820778663166</v>
+        <v>2.3434032378212764</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -8610,7 +8633,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3402558711290427</v>
+        <v>-0.76008968312749581</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -8619,7 +8642,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.57025793151964643</v>
+        <v>0.95598261500164772</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -8628,7 +8651,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.95337537833018382</v>
+        <v>0.45853959488243146</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -8637,7 +8660,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6761834119742376</v>
+        <v>-0.65981418430203442</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -8646,7 +8669,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41962809033921822</v>
+        <v>1.0056392600088764</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -8655,7 +8678,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1555461732531676</v>
+        <v>1.4267779198476243</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -8664,7 +8687,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0324502986536035</v>
+        <v>0.88625156403185001</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -8673,7 +8696,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.8545901234486373E-2</v>
+        <v>0.47626721173020048</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -8682,7 +8705,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48755124380840653</v>
+        <v>0.62298367675079713</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -8691,7 +8714,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18241007590871416</v>
+        <v>-0.57811926669034175</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -8700,7 +8723,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.40645151130854779</v>
+        <v>-0.35823610365033776</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -8709,7 +8732,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.8311490842109572</v>
+        <v>-0.61238002422732263</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -8718,7 +8741,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.96215492498844646</v>
+        <v>-0.18649925450699487</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -8727,7 +8750,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3995494340984942</v>
+        <v>0.81974219397416348</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -8736,7 +8759,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>1.429627205651838</v>
+        <v>0.27356123235836988</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -8745,7 +8768,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46732579014128267</v>
+        <v>-0.64030197339033079</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -8754,7 +8777,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53704066915857618</v>
+        <v>-0.59971385965600577</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -8763,7 +8786,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1793919844635887</v>
+        <v>6.6845541758186314E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -8772,7 +8795,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1105943031094816</v>
+        <v>0.45603723181899752</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -8781,7 +8804,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0122479941224252</v>
+        <v>1.0509898886439115</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -8790,7 +8813,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2253461744283378</v>
+        <v>-1.4983382337419218</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -8799,7 +8822,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.95486093194605204</v>
+        <v>1.7146782835268835</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -8808,7 +8831,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.25488180096545371</v>
+        <v>2.1833898119136865</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -8817,7 +8840,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.87952993905620658</v>
+        <v>0.31201518133058126</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -8826,7 +8849,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0472122627582323</v>
+        <v>-1.3109688270183557</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -8835,7 +8858,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14803438285067375</v>
+        <v>-1.9294154638738026</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -8844,7 +8867,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1002787723627714E-2</v>
+        <v>-0.97504759908101213</v>
       </c>
     </row>
   </sheetData>
@@ -8863,105 +8886,105 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" style="90" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="90" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="90" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="90" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="90" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="90"/>
+    <col min="1" max="1" width="7.140625" style="82" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="82" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="82" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="82" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="82" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="82"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="93" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="89"/>
+      <c r="B1" s="94"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="83" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="92">
+      <c r="A3" s="84">
         <v>217</v>
       </c>
-      <c r="B3" s="93">
+      <c r="B3" s="85">
         <v>41107</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="92">
+      <c r="A4" s="84">
         <v>268</v>
       </c>
-      <c r="B4" s="93">
+      <c r="B4" s="85">
         <v>72707</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="92">
+      <c r="A5" s="84">
         <v>224</v>
       </c>
-      <c r="B5" s="93">
+      <c r="B5" s="85">
         <v>41676</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="92">
+      <c r="A6" s="84">
         <v>286</v>
       </c>
-      <c r="B6" s="93">
+      <c r="B6" s="85">
         <v>87858</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="92">
+      <c r="A7" s="84">
         <v>226</v>
       </c>
-      <c r="B7" s="93">
+      <c r="B7" s="85">
         <v>45606</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="92">
+      <c r="A8" s="84">
         <v>228</v>
       </c>
-      <c r="B8" s="93">
+      <c r="B8" s="85">
         <v>49017</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="92">
+      <c r="A9" s="84">
         <v>234</v>
       </c>
-      <c r="B9" s="93">
+      <c r="B9" s="85">
         <v>57967</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="92">
+      <c r="A10" s="84">
         <v>267</v>
       </c>
-      <c r="B10" s="93">
+      <c r="B10" s="85">
         <v>70702</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="92">
+      <c r="A11" s="84">
         <v>279</v>
       </c>
-      <c r="B11" s="93">
+      <c r="B11" s="85">
         <v>77738</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="92">
+      <c r="A12" s="84">
         <v>261</v>
       </c>
-      <c r="B12" s="93">
+      <c r="B12" s="85">
         <v>69496</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes for CRAN upload
</commit_message>
<xml_diff>
--- a/inst/loadExample.xlsx
+++ b/inst/loadExample.xlsx
@@ -761,11 +761,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185606368"/>
-        <c:axId val="185606928"/>
+        <c:axId val="191519824"/>
+        <c:axId val="191520384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="185606368"/>
+        <c:axId val="191519824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -821,12 +821,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185606928"/>
+        <c:crossAx val="191520384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185606928"/>
+        <c:axId val="191520384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -883,7 +883,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185606368"/>
+        <c:crossAx val="191519824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1194,11 +1194,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="185610848"/>
-        <c:axId val="190716160"/>
+        <c:axId val="191524304"/>
+        <c:axId val="191524864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="185610848"/>
+        <c:axId val="191524304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1241,7 +1241,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190716160"/>
+        <c:crossAx val="191524864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1249,7 +1249,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190716160"/>
+        <c:axId val="191524864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1300,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185610848"/>
+        <c:crossAx val="191524304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1314,7 +1314,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3284,9 +3283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E51"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4286,27 +4283,27 @@
       <c r="F2" s="27"/>
       <c r="I2">
         <f t="shared" ref="I2:N5" ca="1" si="0">RAND()</f>
-        <v>0.22060057268642486</v>
+        <v>8.7531962467226054E-2</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66690748629721264</v>
+        <v>0.62917301559126704</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83671370519404131</v>
+        <v>0.9284323120888478</v>
       </c>
       <c r="L2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7040669797529504E-2</v>
+        <v>0.25531324293453683</v>
       </c>
       <c r="M2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13311669745560573</v>
+        <v>0.37533998259847279</v>
       </c>
       <c r="N2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54117938570305413</v>
+        <v>0.95712694339681037</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
@@ -4317,27 +4314,27 @@
       <c r="F3" s="30"/>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16511433758737537</v>
+        <v>0.14290232312427076</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.528568050784333</v>
+        <v>0.93326491419763846</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94793286774905361</v>
+        <v>0.30414849858785409</v>
       </c>
       <c r="L3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40462046789421091</v>
+        <v>0.52022231509252026</v>
       </c>
       <c r="M3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13151422472851415</v>
+        <v>0.96120707502078695</v>
       </c>
       <c r="N3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88726832638375486</v>
+        <v>0.18003828935577837</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
@@ -4348,27 +4345,27 @@
       <c r="F4" s="30"/>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29213979643112253</v>
+        <v>0.83669213684409327</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86767715374864429</v>
+        <v>0.95736487374263202</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37726136007480926</v>
+        <v>0.19795182492730812</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31002341459144089</v>
+        <v>0.17146390471471906</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3073670969989899</v>
+        <v>0.93239180507298869</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4550588549039354E-3</v>
+        <v>8.4831985021545986E-2</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
@@ -4379,27 +4376,27 @@
       <c r="F5" s="30"/>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49701433143687834</v>
+        <v>0.78731913025155398</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84327755490849365</v>
+        <v>0.85066460882655714</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70596208620789169</v>
+        <v>0.13432198785950555</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="0"/>
-        <v>7.5014691136542799E-2</v>
+        <v>0.74873099481309313</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2451276201868271</v>
+        <v>0.99662805892583983</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3379945012554062</v>
+        <v>5.1049591812333039E-2</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Hyperlink rebuild to handle internal hyperlinks
</commit_message>
<xml_diff>
--- a/inst/loadExample.xlsx
+++ b/inst/loadExample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24525" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24525" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IrisSample" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="30">
   <si>
     <t>Species</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>http://cran.r-project.org/</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -145,6 +142,18 @@
   </si>
   <si>
     <t>Petal Width</t>
+  </si>
+  <si>
+    <t>IrisSample!A1</t>
+  </si>
+  <si>
+    <t>Irrational_number</t>
+  </si>
+  <si>
+    <t>Decimal_fractions</t>
+  </si>
+  <si>
+    <t>IrisSample!A2</t>
   </si>
 </sst>
 </file>
@@ -761,11 +770,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="191519824"/>
-        <c:axId val="191520384"/>
+        <c:axId val="259993904"/>
+        <c:axId val="259996144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="191519824"/>
+        <c:axId val="259993904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -821,12 +830,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191520384"/>
+        <c:crossAx val="259996144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="191520384"/>
+        <c:axId val="259996144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -883,7 +892,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191519824"/>
+        <c:crossAx val="259993904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1194,11 +1203,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="191524304"/>
-        <c:axId val="191524864"/>
+        <c:axId val="260000624"/>
+        <c:axId val="260001184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="191524304"/>
+        <c:axId val="260000624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1241,7 +1250,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191524864"/>
+        <c:crossAx val="260001184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1249,7 +1258,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191524864"/>
+        <c:axId val="260001184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1309,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191524304"/>
+        <c:crossAx val="260000624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3283,7 +3292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3302,16 +3311,16 @@
   <sheetData>
     <row r="1" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>26</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>0</v>
@@ -4264,11 +4273,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q30"/>
+  <dimension ref="B2:Q34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4283,27 +4290,27 @@
       <c r="F2" s="27"/>
       <c r="I2">
         <f t="shared" ref="I2:N5" ca="1" si="0">RAND()</f>
-        <v>8.7531962467226054E-2</v>
+        <v>0.48176569623943455</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62917301559126704</v>
+        <v>0.26951830788963327</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9284323120888478</v>
+        <v>0.87415131933416279</v>
       </c>
       <c r="L2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25531324293453683</v>
+        <v>0.57398289552725368</v>
       </c>
       <c r="M2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37533998259847279</v>
+        <v>1.8975318262670848E-2</v>
       </c>
       <c r="N2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.95712694339681037</v>
+        <v>0.17615264655711538</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
@@ -4314,27 +4321,27 @@
       <c r="F3" s="30"/>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14290232312427076</v>
+        <v>0.49448276072561581</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93326491419763846</v>
+        <v>5.5759425961584119E-2</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30414849858785409</v>
+        <v>0.9486524487835607</v>
       </c>
       <c r="L3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52022231509252026</v>
+        <v>0.41816335639655933</v>
       </c>
       <c r="M3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96120707502078695</v>
+        <v>0.71737738110940263</v>
       </c>
       <c r="N3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18003828935577837</v>
+        <v>0.45690725529415899</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
@@ -4345,27 +4352,27 @@
       <c r="F4" s="30"/>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83669213684409327</v>
+        <v>0.17438427063695772</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.95736487374263202</v>
+        <v>0.81982538145691086</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19795182492730812</v>
+        <v>0.5876877042457731</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17146390471471906</v>
+        <v>1.6510730919371719E-2</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93239180507298869</v>
+        <v>0.34857701433138366</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="0"/>
-        <v>8.4831985021545986E-2</v>
+        <v>0.99876777993196986</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
@@ -4376,27 +4383,27 @@
       <c r="F5" s="30"/>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78731913025155398</v>
+        <v>0.21724113458373739</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85066460882655714</v>
+        <v>0.16280378617517177</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13432198785950555</v>
+        <v>7.1319733260397533E-2</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74873099481309313</v>
+        <v>0.86270757631290851</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99662805892583983</v>
+        <v>0.90215094508329596</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1049591812333039E-2</v>
+        <v>0.57452815477257535</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
@@ -4412,9 +4419,9 @@
       <c r="D7" s="32"/>
       <c r="E7" s="32"/>
       <c r="F7" s="33"/>
-      <c r="I7" s="19" t="s">
-        <v>21</v>
-      </c>
+      <c r="I7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="O7" s="19"/>
     </row>
     <row r="8" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
@@ -4635,7 +4642,7 @@
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
@@ -4646,26 +4653,50 @@
       <c r="F24" s="34"/>
       <c r="G24" s="34"/>
     </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="D26" s="34"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D27" s="34"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D28" s="34"/>
+      <c r="B28" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D29" s="34"/>
+      <c r="B29" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D30" s="34"/>
+      <c r="B30" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="19" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:F7"/>
     <mergeCell ref="B24:G24"/>
-    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="D26:D27"/>
   </mergeCells>
   <conditionalFormatting sqref="I2:N5">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
@@ -4673,11 +4704,17 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="I7" r:id="rId1"/>
+    <hyperlink ref="B25" r:id="rId1"/>
+    <hyperlink ref="B26" r:id="rId2"/>
+    <hyperlink ref="B28" r:id="rId3" location="Decimal_fractions"/>
+    <hyperlink ref="B29" r:id="rId4" location="Decimal_fractions"/>
+    <hyperlink ref="B30" r:id="rId5" location="Decimal_fractions"/>
+    <hyperlink ref="B33" location="IrisSample!A1" display="IrisSample!A1"/>
+    <hyperlink ref="B34" location="IrisSample!A2" display="IrisSample!A2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
maintain diagonal borders on load
</commit_message>
<xml_diff>
--- a/inst/loadExample.xlsx
+++ b/inst/loadExample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24525" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24525" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IrisSample" sheetId="1" r:id="rId1"/>
@@ -216,7 +216,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,8 +229,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -398,12 +404,559 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="6"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="6"/>
+      </right>
+      <top style="medium">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="7" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="7" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </left>
+      <right style="medium">
+        <color theme="7" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color theme="7" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </left>
+      <right style="medium">
+        <color theme="7" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </right>
+      <top style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="5" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="9" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color theme="9" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="mediumDashed">
+        <color theme="9" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color theme="9" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="mediumDashed">
+        <color theme="9" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color theme="9" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color theme="9" tint="-0.249977111117893"/>
+      </right>
+      <top style="mediumDashed">
+        <color theme="9" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color theme="9" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -463,6 +1016,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -770,11 +1364,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="179402928"/>
-        <c:axId val="179403488"/>
+        <c:axId val="177272784"/>
+        <c:axId val="177273328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="179402928"/>
+        <c:axId val="177272784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,12 +1424,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179403488"/>
+        <c:crossAx val="177273328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="179403488"/>
+        <c:axId val="177273328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -892,7 +1486,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179402928"/>
+        <c:crossAx val="177272784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1218,11 +1812,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="179407408"/>
-        <c:axId val="179407968"/>
+        <c:axId val="174339696"/>
+        <c:axId val="174340256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="179407408"/>
+        <c:axId val="174339696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1265,7 +1859,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179407968"/>
+        <c:crossAx val="174340256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1273,7 +1867,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="179407968"/>
+        <c:axId val="174340256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1324,7 +1918,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179407408"/>
+        <c:crossAx val="174339696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1338,7 +1932,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4158,7 +4751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5139,9 +5732,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q34"/>
+  <dimension ref="B2:Q38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5156,27 +5749,27 @@
       <c r="F2" s="25"/>
       <c r="I2">
         <f t="shared" ref="I2:N5" ca="1" si="0">RAND()</f>
-        <v>0.1200098697628279</v>
+        <v>2.1211775296413049E-2</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99941505304699063</v>
+        <v>0.36238269284756286</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33238329441786285</v>
+        <v>0.4179348466232885</v>
       </c>
       <c r="L2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.50935374906320963</v>
+        <v>1.9957991471349912E-3</v>
       </c>
       <c r="M2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43374151260716243</v>
+        <v>0.27074290538522572</v>
       </c>
       <c r="N2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78480884247246463</v>
+        <v>0.2649840322391942</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
@@ -5187,27 +5780,27 @@
       <c r="F3" s="28"/>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1779982427113578E-2</v>
+        <v>0.54173332264029783</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11359390354749566</v>
+        <v>0.38878100760088752</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45161976460862163</v>
+        <v>0.79808537660228029</v>
       </c>
       <c r="L3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5510910412790978</v>
+        <v>0.55660883724632737</v>
       </c>
       <c r="M3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88608414121684409</v>
+        <v>0.66701293339221501</v>
       </c>
       <c r="N3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74070843448639578</v>
+        <v>0.14532555363434596</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
@@ -5218,27 +5811,27 @@
       <c r="F4" s="28"/>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85629450806630725</v>
+        <v>9.5693119051864062E-2</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.90230316078515482</v>
+        <v>0.20964299765376693</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4834637563117079</v>
+        <v>0.86796587246200652</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86608230987280455</v>
+        <v>2.1426862731514396E-2</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.280284896790718</v>
+        <v>0.71629735634319103</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82991252940768745</v>
+        <v>0.76458163284334435</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
@@ -5249,27 +5842,27 @@
       <c r="F5" s="28"/>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74472631567722714</v>
+        <v>0.12078568149512847</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>9.9524787443150964E-2</v>
+        <v>0.60831876756458547</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62328821787698097</v>
+        <v>0.98215511252064946</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30523697689060403</v>
+        <v>0.19344029870818413</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32246177709537016</v>
+        <v>0.32872290981933239</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7046349837130188</v>
+        <v>0.15638833007121067</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
@@ -5530,33 +6123,174 @@
       </c>
       <c r="D26" s="32"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="32"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="D28" s="63"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="64"/>
+      <c r="J28" s="64"/>
+      <c r="K28" s="64"/>
+      <c r="L28" s="64"/>
+      <c r="M28" s="64"/>
+      <c r="N28" s="64"/>
+      <c r="O28" s="64"/>
+      <c r="P28" s="65"/>
+    </row>
+    <row r="29" spans="2:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="D29" s="66"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="56"/>
+      <c r="P29" s="67"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D30" s="66"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="57"/>
+      <c r="O30" s="39"/>
+      <c r="P30" s="67"/>
+    </row>
+    <row r="31" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="66"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="40"/>
+      <c r="P31" s="67"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="D32" s="66"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="58"/>
+      <c r="O32" s="40"/>
+      <c r="P32" s="67"/>
+    </row>
+    <row r="33" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D33" s="66"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="48"/>
+      <c r="L33" s="50"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="58"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="67"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="17" t="s">
         <v>25</v>
       </c>
+      <c r="D34" s="66"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="36"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="58"/>
+      <c r="O34" s="40"/>
+      <c r="P34" s="67"/>
+    </row>
+    <row r="35" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="66"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="60"/>
+      <c r="L35" s="61"/>
+      <c r="M35" s="60"/>
+      <c r="N35" s="60"/>
+      <c r="O35" s="62"/>
+      <c r="P35" s="67"/>
+    </row>
+    <row r="36" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="68"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="69"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="69"/>
+      <c r="J36" s="69"/>
+      <c r="K36" s="69"/>
+      <c r="L36" s="69"/>
+      <c r="M36" s="69"/>
+      <c r="N36" s="69"/>
+      <c r="O36" s="69"/>
+      <c r="P36" s="70"/>
+    </row>
+    <row r="37" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="71"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="72"/>
+      <c r="G38" s="72"/>
+      <c r="H38" s="72"/>
+      <c r="I38" s="72"/>
+      <c r="J38" s="72"/>
+      <c r="K38" s="72"/>
+      <c r="L38" s="72"/>
+      <c r="M38" s="72"/>
+      <c r="N38" s="72"/>
+      <c r="O38" s="72"/>
+      <c r="P38" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>